<commit_message>
add modules and modify some custom code
</commit_message>
<xml_diff>
--- a/PnG_Merchandising/PnGMerchandising.xlsx
+++ b/PnG_Merchandising/PnGMerchandising.xlsx
@@ -5,14 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\PnG_Merchandising\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\(Katalon studio) GitProject\PnG_Merchandising\PnG_Merchandising\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Distribution Region" sheetId="1" r:id="rId1"/>
+    <sheet name="Visit HotSpot" sheetId="2" r:id="rId2"/>
+    <sheet name="Overwrite Hotspot" sheetId="3" r:id="rId3"/>
+    <sheet name="Visit Diapers" sheetId="4" r:id="rId4"/>
+    <sheet name="Overwrite Diapers" sheetId="5" r:id="rId5"/>
+    <sheet name="Visit Hanger" sheetId="6" r:id="rId6"/>
+    <sheet name="Overwrite Hanger " sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>Brand Message</t>
   </si>
@@ -36,15 +42,121 @@
   </si>
   <si>
     <t>Poster</t>
+  </si>
+  <si>
+    <t>Hotspot Available</t>
+  </si>
+  <si>
+    <t>Always Maxi Thicks Extra Long</t>
+  </si>
+  <si>
+    <t>Hotspot Utilization (%)</t>
+  </si>
+  <si>
+    <t>Share Of Shelf</t>
+  </si>
+  <si>
+    <t>Mini ML JP (2)</t>
+  </si>
+  <si>
+    <t>Mini ML MP (2)</t>
+  </si>
+  <si>
+    <t>Midi ML JP (3)</t>
+  </si>
+  <si>
+    <t>Midi ML MP (3)</t>
+  </si>
+  <si>
+    <t>Midi Pants JP (3)</t>
+  </si>
+  <si>
+    <t>Midi Pants MP (3)</t>
+  </si>
+  <si>
+    <t>Maxi ML JP (4)</t>
+  </si>
+  <si>
+    <t>Maxi ML MP (4)</t>
+  </si>
+  <si>
+    <t>Maxi Pants JP (4)</t>
+  </si>
+  <si>
+    <t>Maxi Pants MP (4)</t>
+  </si>
+  <si>
+    <t>Junior ML JP (5)</t>
+  </si>
+  <si>
+    <t>Junior ML MP (5)</t>
+  </si>
+  <si>
+    <t>P&amp;G Others</t>
+  </si>
+  <si>
+    <t>Canbabe</t>
+  </si>
+  <si>
+    <t>Baby Master</t>
+  </si>
+  <si>
+    <t>P&amp;G imported</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Ariel Ariel 45gm</t>
+  </si>
+  <si>
+    <t>Ariel Ariel 95gm</t>
+  </si>
+  <si>
+    <t>H&amp;S Classic Clean 5ml</t>
+  </si>
+  <si>
+    <t>H&amp;S Silky Black 5ml</t>
+  </si>
+  <si>
+    <t>H&amp;S Anti Hair Fall 5ml</t>
+  </si>
+  <si>
+    <t>Pantene Milky Extra Treatment 5ml</t>
+  </si>
+  <si>
+    <t>Utilization (%)</t>
+  </si>
+  <si>
+    <t>Pantene Smooth &amp; Strong 5ml - Sachet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -71,8 +183,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,4 +516,933 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S23"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>18</v>
+      </c>
+      <c r="K2">
+        <v>19</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>21</v>
+      </c>
+      <c r="N2">
+        <v>22</v>
+      </c>
+      <c r="O2">
+        <v>23</v>
+      </c>
+      <c r="P2">
+        <v>24</v>
+      </c>
+      <c r="Q2">
+        <v>25</v>
+      </c>
+      <c r="R2">
+        <v>26</v>
+      </c>
+      <c r="S2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S23"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2">
+        <v>33</v>
+      </c>
+      <c r="F2">
+        <v>34</v>
+      </c>
+      <c r="G2">
+        <v>35</v>
+      </c>
+      <c r="H2">
+        <v>36</v>
+      </c>
+      <c r="I2">
+        <v>37</v>
+      </c>
+      <c r="J2">
+        <v>38</v>
+      </c>
+      <c r="K2">
+        <v>39</v>
+      </c>
+      <c r="L2">
+        <v>40</v>
+      </c>
+      <c r="M2">
+        <v>41</v>
+      </c>
+      <c r="N2">
+        <v>42</v>
+      </c>
+      <c r="O2">
+        <v>43</v>
+      </c>
+      <c r="P2">
+        <v>44</v>
+      </c>
+      <c r="Q2">
+        <v>45</v>
+      </c>
+      <c r="R2">
+        <v>46</v>
+      </c>
+      <c r="S2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>51</v>
+      </c>
+      <c r="D2">
+        <v>52</v>
+      </c>
+      <c r="E2">
+        <v>53</v>
+      </c>
+      <c r="F2">
+        <v>54</v>
+      </c>
+      <c r="G2">
+        <v>55</v>
+      </c>
+      <c r="H2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>61</v>
+      </c>
+      <c r="D2">
+        <v>62</v>
+      </c>
+      <c r="E2">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>64</v>
+      </c>
+      <c r="G2">
+        <v>65</v>
+      </c>
+      <c r="H2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>